<commit_message>
changed to lower level project
</commit_message>
<xml_diff>
--- a/backlog.xlsx
+++ b/backlog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Extra\FYP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8647C5D3-E40F-43E0-A321-67234AE3C743}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B055F2D-C3F7-4EA1-B007-49C7B48BD002}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="53">
   <si>
     <t>ID</t>
   </si>
@@ -53,139 +53,148 @@
     <t>Accesptance crit</t>
   </si>
   <si>
-    <t>Install Unity on laptop</t>
-  </si>
-  <si>
     <t>M</t>
   </si>
   <si>
     <t>Estimate(hr)</t>
   </si>
   <si>
-    <t>unstall unity on latop</t>
-  </si>
-  <si>
-    <t>can start unity on laptop</t>
-  </si>
-  <si>
-    <t>Create project</t>
-  </si>
-  <si>
-    <t>Create a new unity project</t>
-  </si>
-  <si>
-    <t>can open project</t>
-  </si>
-  <si>
-    <t>Create gitlab project</t>
-  </si>
-  <si>
-    <t>Create gitlab page for project</t>
-  </si>
-  <si>
-    <t>gitlab project exists</t>
-  </si>
-  <si>
-    <t>Populate gitlab with backlog</t>
-  </si>
-  <si>
-    <t>Have all backlog ideas in gitlab</t>
-  </si>
-  <si>
-    <t>All backlog items are on gitlab</t>
-  </si>
-  <si>
-    <t>Create quadratic spline tool in unity</t>
-  </si>
-  <si>
-    <t>Follow tutorial to create spline tool</t>
-  </si>
-  <si>
-    <t>Splines can be created with tool in unity</t>
-  </si>
-  <si>
-    <t>Integrate spline tool with mesh renderer</t>
-  </si>
-  <si>
-    <t>Make the spline tool render as a basic mesh</t>
-  </si>
-  <si>
-    <t>Spline tool creates meshes and updates them</t>
-  </si>
-  <si>
-    <t>Recreate paper efficent shader</t>
-  </si>
-  <si>
-    <t>Recreate spline shader described in paper</t>
-  </si>
-  <si>
-    <t>Spline renders as spline and not mesh (curved edges)</t>
-  </si>
-  <si>
-    <t>Create cubic spline tool</t>
-  </si>
-  <si>
     <t>S</t>
   </si>
   <si>
-    <t>Spline tools allows for the creation of cubic curves</t>
-  </si>
-  <si>
-    <t>Recreate paper efficent shader (cubic)</t>
-  </si>
-  <si>
-    <t>Recreate spline shader described in paper with tesselation shader</t>
-  </si>
-  <si>
-    <t>Cubic splines render with cuvred edges</t>
-  </si>
-  <si>
-    <t>Integrate shader to lighting pass</t>
-  </si>
-  <si>
-    <t>Allow for the spline to create shadows</t>
-  </si>
-  <si>
-    <t>Shadows are cast from spline shapes</t>
-  </si>
-  <si>
-    <t>Control shadow strenght</t>
-  </si>
-  <si>
     <t>C</t>
   </si>
   <si>
-    <t>Allow for shadows cast from spline to weaken or remove shadows</t>
-  </si>
-  <si>
-    <t>Spline can remove shadow</t>
-  </si>
-  <si>
-    <t>Create system to animated spline depending on light direction</t>
-  </si>
-  <si>
-    <t>Animate example spline</t>
-  </si>
-  <si>
-    <t>Allow for system to sample animations based on direction</t>
-  </si>
-  <si>
-    <t>Light direction now changes the shape and shade of spline</t>
-  </si>
-  <si>
-    <t>Create example spline shadow shading mesh</t>
-  </si>
-  <si>
-    <t>Can play example realtime</t>
-  </si>
-  <si>
-    <t>Make playable controller</t>
-  </si>
-  <si>
-    <t>Create a controllable player character with spline shadow</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Users can now control a spline </t>
+    <t>Set up C++ IDE</t>
+  </si>
+  <si>
+    <t>Set up IDE for C++ development</t>
+  </si>
+  <si>
+    <t>Can complie hello world.cpp</t>
+  </si>
+  <si>
+    <t>Add libraries to project</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Intigrate Vulkan SDK and windowing library </t>
+  </si>
+  <si>
+    <t>Library can be used in C++ code</t>
+  </si>
+  <si>
+    <t>Create window hello world</t>
+  </si>
+  <si>
+    <t>Create program to create coloured window</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Window with clear colour </t>
+  </si>
+  <si>
+    <t>Have triangle show up</t>
+  </si>
+  <si>
+    <t>alter program to have triangle show up in window</t>
+  </si>
+  <si>
+    <t>Window now features a tri colour triangle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Load mesh </t>
+  </si>
+  <si>
+    <t>Have mesh file loaded into the program</t>
+  </si>
+  <si>
+    <t>Window now shows abutraty loaded mesh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Load svg </t>
+  </si>
+  <si>
+    <t>Have SVG into program</t>
+  </si>
+  <si>
+    <t>Abutrary SVG displays on screen as mesh</t>
+  </si>
+  <si>
+    <t>Have SVG have shaders apply to display curves</t>
+  </si>
+  <si>
+    <t>SVGs have curves instead of straight edges</t>
+  </si>
+  <si>
+    <t>SVG algorithm</t>
+  </si>
+  <si>
+    <t>Lighting pass</t>
+  </si>
+  <si>
+    <t>Add lighting pass</t>
+  </si>
+  <si>
+    <t>Create scene</t>
+  </si>
+  <si>
+    <t>Place plane and cube in scene with SVG</t>
+  </si>
+  <si>
+    <t>Display renders floor, cube and SVG</t>
+  </si>
+  <si>
+    <t>Cube, SVG and plane are lit</t>
+  </si>
+  <si>
+    <t>Shadow map</t>
+  </si>
+  <si>
+    <t>Add Shadow pass</t>
+  </si>
+  <si>
+    <t>Have Cube and SVG cast shadows</t>
+  </si>
+  <si>
+    <t>Shadow strenght variance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Have SVG not render </t>
+  </si>
+  <si>
+    <t>Have SVG only cast shadow</t>
+  </si>
+  <si>
+    <t>Spline animation</t>
+  </si>
+  <si>
+    <t>Allow for lerping splines</t>
+  </si>
+  <si>
+    <t>Have spline change shape</t>
+  </si>
+  <si>
+    <t>Have shadow strenght animate</t>
+  </si>
+  <si>
+    <t>Have shadow strenght change</t>
+  </si>
+  <si>
+    <t>base animation on light rotation</t>
+  </si>
+  <si>
+    <t>base animations on Slerping on light rotation</t>
+  </si>
+  <si>
+    <t>Have light rotation be controllable</t>
+  </si>
+  <si>
+    <t>Add controller based on key inputs to change light direction</t>
+  </si>
+  <si>
+    <t>Light roation can be changed with time</t>
+  </si>
+  <si>
+    <t>Light rotation changes spline shape and shadow strenght</t>
   </si>
 </sst>
 </file>
@@ -523,10 +532,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -550,7 +559,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>3</v>
@@ -565,40 +574,40 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
       <c r="D2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E2" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="F2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3">
-        <f t="shared" ref="A3:A22" si="0">ROW(A2)</f>
+        <f t="shared" ref="A3:A15" si="0">ROW(A2)</f>
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E3" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="F3" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -607,19 +616,19 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E4" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F4" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -628,19 +637,19 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E5" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="F5" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
@@ -649,19 +658,19 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E6" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="F6" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -670,19 +679,19 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D7">
         <v>2</v>
       </c>
       <c r="E7" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="F7" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
@@ -691,19 +700,19 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="C8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D8">
         <v>2</v>
       </c>
       <c r="E8" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F8" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
@@ -712,19 +721,19 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="C9" t="s">
-        <v>29</v>
+        <v>7</v>
       </c>
       <c r="D9">
         <v>2</v>
       </c>
       <c r="E9" t="s">
-        <v>20</v>
+        <v>33</v>
       </c>
       <c r="F9" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
@@ -733,19 +742,19 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10">
+        <v>2</v>
+      </c>
+      <c r="E10" t="s">
         <v>31</v>
       </c>
-      <c r="C10" t="s">
-        <v>29</v>
-      </c>
-      <c r="D10">
-        <v>2</v>
-      </c>
-      <c r="E10" t="s">
-        <v>32</v>
-      </c>
       <c r="F10" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
@@ -754,19 +763,19 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C11" t="s">
-        <v>29</v>
+        <v>7</v>
       </c>
       <c r="D11">
         <v>2</v>
       </c>
       <c r="E11" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="F11" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
@@ -775,19 +784,19 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C12" t="s">
-        <v>38</v>
+        <v>8</v>
       </c>
       <c r="D12">
         <v>2</v>
       </c>
       <c r="E12" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F12" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
@@ -796,10 +805,10 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C13" t="s">
-        <v>38</v>
+        <v>8</v>
       </c>
       <c r="D13">
         <v>2</v>
@@ -817,16 +826,16 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="C14" t="s">
-        <v>38</v>
+        <v>8</v>
       </c>
       <c r="D14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E14" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="F14" t="s">
         <v>46</v>
@@ -841,7 +850,7 @@
         <v>47</v>
       </c>
       <c r="C15" t="s">
-        <v>38</v>
+        <v>8</v>
       </c>
       <c r="D15">
         <v>2</v>
@@ -850,7 +859,27 @@
         <v>48</v>
       </c>
       <c r="F15" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
         <v>49</v>
+      </c>
+      <c r="C16" t="s">
+        <v>8</v>
+      </c>
+      <c r="D16">
+        <v>2</v>
+      </c>
+      <c r="E16" t="s">
+        <v>50</v>
+      </c>
+      <c r="F16" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>